<commit_message>
First modifications in the pipeline and handler
</commit_message>
<xml_diff>
--- a/simulation_data/Masterfile.xlsx
+++ b/simulation_data/Masterfile.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t xml:space="preserve">PARAMETER</t>
   </si>
@@ -50,6 +50,18 @@
   </si>
   <si>
     <t xml:space="preserve">postProcessing/probes/0/p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mesher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blockMesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">simpleFoam</t>
   </si>
   <si>
     <t xml:space="preserve">VARIABLE</t>
@@ -224,10 +236,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -273,6 +285,22 @@
       </c>
       <c r="B5" s="0" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -305,30 +333,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
@@ -342,10 +370,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>100</v>
@@ -359,13 +387,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -411,18 +439,18 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>5</v>
@@ -433,7 +461,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>10</v>
@@ -444,7 +472,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1000</v>
@@ -486,33 +514,33 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
@@ -527,15 +555,15 @@
         <v>2</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>10000</v>

</xml_diff>

<commit_message>
Major improvements: 1. Master/Variant/Resultfile in simulation_data dictionary, 2. OF case in openfoam_case dictionary, 3. Cleaning of openfoam_case dictionary after use, 4. mesher and solver are read from the Masterfile.xlsx. All changes tested successfully.
</commit_message>
<xml_diff>
--- a/simulation_data/Masterfile.xlsx
+++ b/simulation_data/Masterfile.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">output_file</t>
   </si>
   <si>
-    <t xml:space="preserve">postProcessing/probes/0/p</t>
+    <t xml:space="preserve">/postProcessing/probes/0/p</t>
   </si>
   <si>
     <t xml:space="preserve">mesher</t>
@@ -239,7 +239,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>